<commit_message>
population analysis - diversity index & descriptive statistics
</commit_message>
<xml_diff>
--- a/PROJECTS/Population/Dataset_pop/States_pop.xlsx
+++ b/PROJECTS/Population/Dataset_pop/States_pop.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb775b60f7163cde/Desktop/DATASET/POPULATION/STATES_csv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASYIKIN\OneDrive\Desktop\PYTHON FOR DATA ANALYSIS\PROJECTS\Population\Dataset_pop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="305" documentId="8_{6F1BD218-AF57-4C64-B2D3-70F370FAEFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0CE1AED-8B36-47BA-8047-331DD5BC9EE9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAE5675-74F7-470A-AA7B-3811CD5C8FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="912" xr2:uid="{CB78915E-DD85-44B7-BB1E-376C6780AB3F}"/>
+    <workbookView xWindow="-15458" yWindow="-3570" windowWidth="15556" windowHeight="11715" tabRatio="912" firstSheet="1" activeTab="14" xr2:uid="{CB78915E-DD85-44B7-BB1E-376C6780AB3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="16" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="36">
   <si>
     <t>Year</t>
   </si>
@@ -141,6 +141,24 @@
   <si>
     <t>(1000s)</t>
   </si>
+  <si>
+    <t>1980-1990</t>
+  </si>
+  <si>
+    <t>https://pqi.stats.gov.my/result.php?token=3f75052bf33e6faa7836fd08ce3dc754</t>
+  </si>
+  <si>
+    <t>1991-1999</t>
+  </si>
+  <si>
+    <t>https://pqi.stats.gov.my/result.php?token=df8278616ef180a270562757e0e2cac0</t>
+  </si>
+  <si>
+    <t>2000-2010</t>
+  </si>
+  <si>
+    <t>https://pqi.stats.gov.my/result.php?token=e4488542fe6e0634f4e4ff43d22e04b6</t>
+  </si>
 </sst>
 </file>
 
@@ -158,7 +176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,7 +197,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -235,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -270,11 +294,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4544,7 +4570,7 @@
                   <c:v>1995</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1986</c:v>
+                  <c:v>1996</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1997</c:v>
@@ -6145,16 +6171,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>358775</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>225425</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>53975</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>15875</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>530225</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6180,10 +6206,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6485,8 +6507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746B3F18-905E-441E-8BD1-48B44ECBDFA2}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -6535,7 +6557,7 @@
       <c r="N1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8468,36 +8490,36 @@
       <c r="P42" s="6"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13344,7 +13366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBBA1813-83C3-465B-8B88-AAFEA1DBA0A5}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -16312,20 +16334,20 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA60960F-2D71-4925-853E-984328F82620}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13:L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="8.7265625" style="12"/>
-    <col min="10" max="10" width="8.7265625" style="12"/>
+    <col min="7" max="8" width="8.7265625" style="16"/>
+    <col min="11" max="11" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16344,23 +16366,26 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1980</v>
       </c>
@@ -16379,20 +16404,26 @@
       <c r="F2">
         <v>200.6</v>
       </c>
-      <c r="G2" s="12">
-        <v>5.2</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="I2">
         <v>468.2</v>
       </c>
-      <c r="I2">
-        <v>81.3</v>
-      </c>
-      <c r="J2" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <v>194.1</v>
+      </c>
+      <c r="K2" s="14">
+        <v>1.6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1981</v>
       </c>
@@ -16411,20 +16442,26 @@
       <c r="F3">
         <v>205.2</v>
       </c>
-      <c r="G3" s="12">
-        <v>5.5</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="I3">
         <v>476.8</v>
       </c>
-      <c r="I3">
-        <v>83.6</v>
-      </c>
-      <c r="J3" s="12">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <v>198</v>
+      </c>
+      <c r="K3" s="14">
+        <v>1.6</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1982</v>
       </c>
@@ -16443,20 +16480,26 @@
       <c r="F4">
         <v>209.6</v>
       </c>
-      <c r="G4" s="12">
-        <v>5.8</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I4">
         <v>486.1</v>
       </c>
-      <c r="I4">
-        <v>85.9</v>
-      </c>
-      <c r="J4" s="12">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <v>201.7</v>
+      </c>
+      <c r="K4" s="14">
+        <v>1.6</v>
+      </c>
+      <c r="O4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1983</v>
       </c>
@@ -16475,20 +16518,20 @@
       <c r="F5">
         <v>213.9</v>
       </c>
-      <c r="G5" s="12">
-        <v>6.1</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I5">
         <v>495.8</v>
       </c>
-      <c r="I5">
-        <v>88</v>
-      </c>
-      <c r="J5" s="12">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <v>205.2</v>
+      </c>
+      <c r="K5" s="14">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1984</v>
       </c>
@@ -16507,20 +16550,20 @@
       <c r="F6">
         <v>218</v>
       </c>
-      <c r="G6" s="12">
-        <v>6.4</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="14">
+        <v>2.4</v>
+      </c>
+      <c r="I6">
         <v>505.7</v>
       </c>
-      <c r="I6">
-        <v>90.3</v>
-      </c>
-      <c r="J6" s="12">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <v>208.4</v>
+      </c>
+      <c r="K6" s="14">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1985</v>
       </c>
@@ -16539,20 +16582,20 @@
       <c r="F7">
         <v>222.3</v>
       </c>
-      <c r="G7" s="12">
-        <v>6.6</v>
-      </c>
-      <c r="H7">
+      <c r="G7" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="I7">
         <v>516.4</v>
       </c>
-      <c r="I7">
-        <v>92.5</v>
-      </c>
-      <c r="J7" s="12">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <v>212</v>
+      </c>
+      <c r="K7" s="14">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1986</v>
       </c>
@@ -16571,20 +16614,20 @@
       <c r="F8">
         <v>226.5</v>
       </c>
-      <c r="G8" s="12">
-        <v>6.9</v>
-      </c>
-      <c r="H8">
+      <c r="G8" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="I8">
         <v>528.79999999999995</v>
       </c>
-      <c r="I8">
-        <v>94.7</v>
-      </c>
-      <c r="J8" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>215.5</v>
+      </c>
+      <c r="K8" s="14">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1987</v>
       </c>
@@ -16603,20 +16646,20 @@
       <c r="F9">
         <v>230.8</v>
       </c>
-      <c r="G9" s="12">
-        <v>7.2</v>
-      </c>
-      <c r="H9">
+      <c r="G9" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="I9">
         <v>541.4</v>
       </c>
-      <c r="I9">
-        <v>96.6</v>
-      </c>
-      <c r="J9" s="12">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J9">
+        <v>218.6</v>
+      </c>
+      <c r="K9" s="14">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1988</v>
       </c>
@@ -16635,20 +16678,20 @@
       <c r="F10">
         <v>235.3</v>
       </c>
-      <c r="G10" s="12">
-        <v>7.5</v>
-      </c>
-      <c r="H10">
+      <c r="G10" s="14">
+        <v>2.7</v>
+      </c>
+      <c r="I10">
         <v>555.1</v>
       </c>
-      <c r="I10">
-        <v>98.6</v>
-      </c>
-      <c r="J10" s="12">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J10">
+        <v>222.2</v>
+      </c>
+      <c r="K10" s="14">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1989</v>
       </c>
@@ -16667,20 +16710,20 @@
       <c r="F11">
         <v>240</v>
       </c>
-      <c r="G11" s="12">
-        <v>7.8</v>
-      </c>
-      <c r="H11">
+      <c r="G11" s="14">
+        <v>2.8</v>
+      </c>
+      <c r="I11">
         <v>568.5</v>
       </c>
-      <c r="I11">
-        <v>100.8</v>
-      </c>
-      <c r="J11" s="12">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J11">
+        <v>226</v>
+      </c>
+      <c r="K11" s="14">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1990</v>
       </c>
@@ -16699,20 +16742,20 @@
       <c r="F12">
         <v>243.6</v>
       </c>
-      <c r="G12" s="12">
-        <v>8</v>
-      </c>
-      <c r="H12">
+      <c r="G12" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="I12">
         <v>581.1</v>
       </c>
-      <c r="I12">
-        <v>102.9</v>
-      </c>
-      <c r="J12" s="12">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J12">
+        <v>229</v>
+      </c>
+      <c r="K12" s="14">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1991</v>
       </c>
@@ -16729,22 +16772,28 @@
         <v>494.5</v>
       </c>
       <c r="F13">
-        <v>260.8</v>
-      </c>
-      <c r="G13" s="12">
-        <v>5.8</v>
-      </c>
-      <c r="H13">
+        <v>247.3</v>
+      </c>
+      <c r="G13" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="H13" s="16">
+        <v>1.7</v>
+      </c>
+      <c r="I13">
         <v>284.8</v>
       </c>
-      <c r="I13">
-        <v>170.7</v>
-      </c>
-      <c r="J13" s="12">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J13">
+        <v>232</v>
+      </c>
+      <c r="K13" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="L13" s="15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1992</v>
       </c>
@@ -16761,22 +16810,28 @@
         <v>503.1</v>
       </c>
       <c r="F14">
-        <v>265</v>
-      </c>
-      <c r="G14" s="12">
-        <v>5.4</v>
-      </c>
-      <c r="H14">
+        <v>251</v>
+      </c>
+      <c r="G14" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="H14" s="16">
+        <v>1.8</v>
+      </c>
+      <c r="I14">
         <v>287.7</v>
       </c>
-      <c r="I14">
-        <v>178.7</v>
-      </c>
-      <c r="J14" s="12">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J14">
+        <v>234.1</v>
+      </c>
+      <c r="K14" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="L14" s="15">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1993</v>
       </c>
@@ -16793,22 +16848,28 @@
         <v>511.9</v>
       </c>
       <c r="F15">
-        <v>269</v>
-      </c>
-      <c r="G15" s="12">
-        <v>5.5</v>
-      </c>
-      <c r="H15">
+        <v>254.4</v>
+      </c>
+      <c r="G15" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="H15" s="16">
+        <v>1.9</v>
+      </c>
+      <c r="I15">
         <v>292</v>
       </c>
-      <c r="I15">
-        <v>186.7</v>
-      </c>
-      <c r="J15" s="12">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J15">
+        <v>237.7</v>
+      </c>
+      <c r="K15" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L15" s="15">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1994</v>
       </c>
@@ -16825,22 +16886,28 @@
         <v>520.79999999999995</v>
       </c>
       <c r="F16">
-        <v>273.2</v>
-      </c>
-      <c r="G16" s="12">
-        <v>5.6</v>
-      </c>
-      <c r="H16">
+        <v>257.8</v>
+      </c>
+      <c r="G16" s="15">
+        <v>2.7</v>
+      </c>
+      <c r="H16" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="I16">
         <v>296.5</v>
       </c>
-      <c r="I16">
-        <v>194.7</v>
-      </c>
-      <c r="J16" s="12">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J16">
+        <v>241.2</v>
+      </c>
+      <c r="K16" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L16" s="15">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1995</v>
       </c>
@@ -16857,24 +16924,30 @@
         <v>529</v>
       </c>
       <c r="F17">
-        <v>277.3</v>
-      </c>
-      <c r="G17" s="12">
-        <v>5.7</v>
-      </c>
-      <c r="H17">
+        <v>261</v>
+      </c>
+      <c r="G17" s="15">
+        <v>2.6</v>
+      </c>
+      <c r="H17" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="I17">
         <v>300.60000000000002</v>
       </c>
-      <c r="I17">
-        <v>202.7</v>
-      </c>
-      <c r="J17" s="12">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J17">
+        <v>244.6</v>
+      </c>
+      <c r="K17" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L17" s="15">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>1986</v>
+        <v>1996</v>
       </c>
       <c r="B18">
         <v>1904.5</v>
@@ -16889,22 +16962,28 @@
         <v>537.29999999999995</v>
       </c>
       <c r="F18">
-        <v>281.5</v>
-      </c>
-      <c r="G18" s="12">
-        <v>5.7</v>
-      </c>
-      <c r="H18">
+        <v>264</v>
+      </c>
+      <c r="G18" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="H18" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="I18">
         <v>304.7</v>
       </c>
-      <c r="I18">
-        <v>210.7</v>
-      </c>
-      <c r="J18" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J18">
+        <v>247.8</v>
+      </c>
+      <c r="K18" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L18" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1997</v>
       </c>
@@ -16921,22 +17000,28 @@
         <v>546</v>
       </c>
       <c r="F19">
-        <v>285.89999999999998</v>
-      </c>
-      <c r="G19" s="12">
-        <v>5.8</v>
-      </c>
-      <c r="H19">
+        <v>266.8</v>
+      </c>
+      <c r="G19" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="H19" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="I19">
         <v>308.8</v>
       </c>
-      <c r="I19">
-        <v>218.5</v>
-      </c>
-      <c r="J19" s="12">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J19">
+        <v>251.1</v>
+      </c>
+      <c r="K19" s="15">
+        <v>1.9</v>
+      </c>
+      <c r="L19" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1998</v>
       </c>
@@ -16953,22 +17038,28 @@
         <v>554.70000000000005</v>
       </c>
       <c r="F20">
-        <v>290.8</v>
-      </c>
-      <c r="G20" s="12">
-        <v>5.8</v>
-      </c>
-      <c r="H20">
+        <v>269.5</v>
+      </c>
+      <c r="G20" s="15">
+        <v>2.4</v>
+      </c>
+      <c r="H20" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="I20">
         <v>312.89999999999998</v>
       </c>
-      <c r="I20">
-        <v>226.2</v>
-      </c>
-      <c r="J20" s="12">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J20">
+        <v>254.3</v>
+      </c>
+      <c r="K20" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="L20" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1999</v>
       </c>
@@ -16985,22 +17076,28 @@
         <v>564.09999999999991</v>
       </c>
       <c r="F21">
-        <v>296.2</v>
-      </c>
-      <c r="G21" s="12">
-        <v>5.9</v>
-      </c>
-      <c r="H21">
+        <v>272.3</v>
+      </c>
+      <c r="G21" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H21" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="I21">
         <v>317.39999999999998</v>
       </c>
-      <c r="I21">
-        <v>233.8</v>
-      </c>
-      <c r="J21" s="12">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J21">
+        <v>257.8</v>
+      </c>
+      <c r="K21" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="L21" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2000</v>
       </c>
@@ -17017,22 +17114,28 @@
         <v>574.5</v>
       </c>
       <c r="F22">
-        <v>302.5</v>
-      </c>
-      <c r="G22" s="12">
-        <v>5.6</v>
-      </c>
-      <c r="H22">
+        <v>275.3</v>
+      </c>
+      <c r="G22" s="14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H22" s="16">
+        <v>2.1</v>
+      </c>
+      <c r="I22">
         <v>322.7</v>
       </c>
-      <c r="I22">
-        <v>241.1</v>
-      </c>
-      <c r="J22" s="12">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J22">
+        <v>261.89999999999998</v>
+      </c>
+      <c r="K22" s="14">
+        <v>1.8</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2001</v>
       </c>
@@ -17049,22 +17152,28 @@
         <v>586.4</v>
       </c>
       <c r="F23">
-        <v>308.2</v>
-      </c>
-      <c r="G23" s="12">
-        <v>5.6</v>
-      </c>
-      <c r="H23">
+        <v>279.39999999999998</v>
+      </c>
+      <c r="G23" s="14">
+        <v>2.4</v>
+      </c>
+      <c r="H23" s="16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I23">
         <v>328.6</v>
       </c>
-      <c r="I23">
-        <v>245</v>
-      </c>
-      <c r="J23" s="12">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J23">
+        <v>265.39999999999998</v>
+      </c>
+      <c r="K23" s="14">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2002</v>
       </c>
@@ -17081,22 +17190,28 @@
         <v>597.5</v>
       </c>
       <c r="F24">
-        <v>313.7</v>
-      </c>
-      <c r="G24" s="12">
-        <v>5.5</v>
-      </c>
-      <c r="H24">
+        <v>282.7</v>
+      </c>
+      <c r="G24" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="H24" s="16">
+        <v>2.4</v>
+      </c>
+      <c r="I24">
         <v>333.4</v>
       </c>
-      <c r="I24">
-        <v>248.5</v>
-      </c>
-      <c r="J24" s="12">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J24">
+        <v>268</v>
+      </c>
+      <c r="K24" s="14">
+        <v>2.1</v>
+      </c>
+      <c r="L24">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2003</v>
       </c>
@@ -17113,22 +17228,28 @@
         <v>607.5</v>
       </c>
       <c r="F25">
-        <v>319.39999999999998</v>
-      </c>
-      <c r="G25" s="12">
-        <v>5.5</v>
-      </c>
-      <c r="H25">
+        <v>285.7</v>
+      </c>
+      <c r="G25" s="14">
+        <v>2.7</v>
+      </c>
+      <c r="H25" s="16">
+        <v>2.5</v>
+      </c>
+      <c r="I25">
         <v>337.8</v>
       </c>
-      <c r="I25">
-        <v>251.7</v>
-      </c>
-      <c r="J25" s="12">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J25">
+        <v>270.3</v>
+      </c>
+      <c r="K25" s="14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L25">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2004</v>
       </c>
@@ -17145,22 +17266,28 @@
         <v>617.40000000000009</v>
       </c>
       <c r="F26">
-        <v>324.89999999999998</v>
-      </c>
-      <c r="G26" s="12">
-        <v>5.4</v>
-      </c>
-      <c r="H26">
+        <v>288.39999999999998</v>
+      </c>
+      <c r="G26" s="14">
+        <v>2.9</v>
+      </c>
+      <c r="H26" s="16">
+        <v>2.6</v>
+      </c>
+      <c r="I26">
         <v>342</v>
       </c>
-      <c r="I26">
-        <v>255.3</v>
-      </c>
-      <c r="J26" s="12">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J26">
+        <v>272.5</v>
+      </c>
+      <c r="K26" s="14">
+        <v>2.4</v>
+      </c>
+      <c r="L26">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2005</v>
       </c>
@@ -17177,22 +17304,28 @@
         <v>627.6</v>
       </c>
       <c r="F27">
-        <v>330.9</v>
-      </c>
-      <c r="G27" s="12">
-        <v>5.4</v>
-      </c>
-      <c r="H27">
+        <v>290.89999999999998</v>
+      </c>
+      <c r="G27" s="14">
+        <v>3.1</v>
+      </c>
+      <c r="H27" s="16">
+        <v>2.8</v>
+      </c>
+      <c r="I27">
         <v>346.2</v>
       </c>
-      <c r="I27">
-        <v>259.10000000000002</v>
-      </c>
-      <c r="J27" s="12">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J27">
+        <v>274.5</v>
+      </c>
+      <c r="K27" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="L27">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2006</v>
       </c>
@@ -17209,22 +17342,28 @@
         <v>638</v>
       </c>
       <c r="F28">
-        <v>336.9</v>
-      </c>
-      <c r="G28" s="12">
-        <v>5.3</v>
-      </c>
-      <c r="H28">
+        <v>293.39999999999998</v>
+      </c>
+      <c r="G28" s="14">
+        <v>3.2</v>
+      </c>
+      <c r="H28" s="16">
+        <v>3.1</v>
+      </c>
+      <c r="I28">
         <v>350.6</v>
       </c>
-      <c r="I28">
-        <v>263.10000000000002</v>
-      </c>
-      <c r="J28" s="12">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J28">
+        <v>276.5</v>
+      </c>
+      <c r="K28" s="14">
+        <v>2.8</v>
+      </c>
+      <c r="L28">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2007</v>
       </c>
@@ -17241,22 +17380,28 @@
         <v>648.5</v>
       </c>
       <c r="F29">
-        <v>342.3</v>
-      </c>
-      <c r="G29" s="12">
-        <v>5.3</v>
-      </c>
-      <c r="H29">
+        <v>295.60000000000002</v>
+      </c>
+      <c r="G29" s="14">
+        <v>3.4</v>
+      </c>
+      <c r="H29" s="16">
+        <v>3.4</v>
+      </c>
+      <c r="I29">
         <v>354.9</v>
       </c>
-      <c r="I29">
-        <v>267.3</v>
-      </c>
-      <c r="J29" s="12">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J29">
+        <v>278.10000000000002</v>
+      </c>
+      <c r="K29" s="14">
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2008</v>
       </c>
@@ -17273,22 +17418,28 @@
         <v>659</v>
       </c>
       <c r="F30">
-        <v>348.4</v>
-      </c>
-      <c r="G30" s="12">
-        <v>5.2</v>
-      </c>
-      <c r="H30">
+        <v>298</v>
+      </c>
+      <c r="G30" s="14">
+        <v>3.6</v>
+      </c>
+      <c r="H30" s="16">
+        <v>3.8</v>
+      </c>
+      <c r="I30">
         <v>359.1</v>
       </c>
-      <c r="I30">
-        <v>271.89999999999998</v>
-      </c>
-      <c r="J30" s="12">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J30">
+        <v>279.7</v>
+      </c>
+      <c r="K30" s="14">
+        <v>3.2</v>
+      </c>
+      <c r="L30">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2009</v>
       </c>
@@ -17305,22 +17456,28 @@
         <v>669</v>
       </c>
       <c r="F31">
-        <v>354.6</v>
-      </c>
-      <c r="G31" s="12">
-        <v>5.2</v>
-      </c>
-      <c r="H31">
+        <v>300</v>
+      </c>
+      <c r="G31" s="14">
+        <v>3.8</v>
+      </c>
+      <c r="H31" s="16">
+        <v>4.2</v>
+      </c>
+      <c r="I31">
         <v>363.1</v>
       </c>
-      <c r="I31">
-        <v>276.7</v>
-      </c>
-      <c r="J31" s="12">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J31">
+        <v>281.2</v>
+      </c>
+      <c r="K31" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="L31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2010</v>
       </c>
@@ -17339,20 +17496,26 @@
       <c r="F32">
         <v>301.60000000000002</v>
       </c>
-      <c r="G32" s="12">
-        <v>5.2</v>
-      </c>
-      <c r="H32">
+      <c r="G32" s="14">
+        <v>3.9</v>
+      </c>
+      <c r="H32" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="I32">
         <v>592.5</v>
       </c>
-      <c r="I32">
-        <v>142.4</v>
-      </c>
-      <c r="J32" s="12">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J32">
+        <v>282.5</v>
+      </c>
+      <c r="K32" s="14">
+        <v>3.5</v>
+      </c>
+      <c r="L32">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -17371,20 +17534,13 @@
       <c r="F33">
         <v>304.39999999999998</v>
       </c>
-      <c r="G33" s="12">
-        <v>5.7</v>
-      </c>
-      <c r="H33">
+      <c r="G33" s="15"/>
+      <c r="I33">
         <v>603.29999999999995</v>
       </c>
-      <c r="I33">
-        <v>143.69999999999999</v>
-      </c>
-      <c r="J33" s="12">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K33" s="15"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2012</v>
       </c>
@@ -17403,20 +17559,13 @@
       <c r="F34">
         <v>307.7</v>
       </c>
-      <c r="G34" s="12">
-        <v>6</v>
-      </c>
-      <c r="H34">
+      <c r="G34" s="15"/>
+      <c r="I34">
         <v>611.1</v>
       </c>
-      <c r="I34">
-        <v>144.5</v>
-      </c>
-      <c r="J34" s="12">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K34" s="15"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2013</v>
       </c>
@@ -17435,20 +17584,13 @@
       <c r="F35">
         <v>311.10000000000002</v>
       </c>
-      <c r="G35" s="12">
-        <v>6.7</v>
-      </c>
-      <c r="H35">
+      <c r="G35" s="15"/>
+      <c r="I35">
         <v>619</v>
       </c>
-      <c r="I35">
-        <v>145.1</v>
-      </c>
-      <c r="J35" s="12">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K35" s="15"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2014</v>
       </c>
@@ -17467,20 +17609,13 @@
       <c r="F36">
         <v>313.10000000000002</v>
       </c>
-      <c r="G36" s="12">
-        <v>6.7</v>
-      </c>
-      <c r="H36">
+      <c r="G36" s="15"/>
+      <c r="I36">
         <v>628.29999999999995</v>
       </c>
-      <c r="I36">
-        <v>146.4</v>
-      </c>
-      <c r="J36" s="12">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K36" s="15"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2015</v>
       </c>
@@ -17499,20 +17634,13 @@
       <c r="F37">
         <v>315.5</v>
       </c>
-      <c r="G37" s="12">
-        <v>6.7</v>
-      </c>
-      <c r="H37">
+      <c r="G37" s="15"/>
+      <c r="I37">
         <v>636.20000000000005</v>
       </c>
-      <c r="I37">
-        <v>146.6</v>
-      </c>
-      <c r="J37" s="12">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K37" s="15"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2016</v>
       </c>
@@ -17531,20 +17659,13 @@
       <c r="F38">
         <v>317.39999999999998</v>
       </c>
-      <c r="G38" s="12">
-        <v>6.8</v>
-      </c>
-      <c r="H38">
+      <c r="G38" s="15"/>
+      <c r="I38">
         <v>645</v>
       </c>
-      <c r="I38">
-        <v>148.5</v>
-      </c>
-      <c r="J38" s="12">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K38" s="15"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2017</v>
       </c>
@@ -17563,20 +17684,13 @@
       <c r="F39">
         <v>318.89999999999998</v>
       </c>
-      <c r="G39" s="12">
-        <v>7.2</v>
-      </c>
-      <c r="H39">
+      <c r="G39" s="15"/>
+      <c r="I39">
         <v>651.29999999999995</v>
       </c>
-      <c r="I39">
-        <v>148.5</v>
-      </c>
-      <c r="J39" s="12">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K39" s="15"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2018</v>
       </c>
@@ -17595,20 +17709,13 @@
       <c r="F40">
         <v>320.2</v>
       </c>
-      <c r="G40" s="12">
-        <v>7.2</v>
-      </c>
-      <c r="H40">
+      <c r="G40" s="15"/>
+      <c r="I40">
         <v>657.6</v>
       </c>
-      <c r="I40">
-        <v>148.69999999999999</v>
-      </c>
-      <c r="J40" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K40" s="15"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2019</v>
       </c>
@@ -17627,20 +17734,13 @@
       <c r="F41">
         <v>321.5</v>
       </c>
-      <c r="G41" s="12">
-        <v>7.2</v>
-      </c>
-      <c r="H41">
+      <c r="G41" s="15"/>
+      <c r="I41">
         <v>663.6</v>
       </c>
-      <c r="I41">
-        <v>148.9</v>
-      </c>
-      <c r="J41" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K41" s="15"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2020</v>
       </c>
@@ -17659,18 +17759,11 @@
       <c r="F42">
         <v>285.39999999999998</v>
       </c>
-      <c r="G42" s="12">
-        <v>3.4</v>
-      </c>
-      <c r="H42">
+      <c r="G42" s="15"/>
+      <c r="I42">
         <v>587.6</v>
       </c>
-      <c r="I42">
-        <v>117.3</v>
-      </c>
-      <c r="J42" s="12">
-        <v>2.6</v>
-      </c>
+      <c r="K42" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19765,8 +19858,8 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O51" sqref="O51"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19814,7 +19907,7 @@
       <c r="N1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -21749,20 +21842,20 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B44">
@@ -21812,59 +21905,59 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B45" s="14">
+      <c r="B45" s="13">
         <f>B44-B41</f>
         <v>248.5</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C45" s="13">
         <f t="shared" ref="C45:O45" si="0">C44-C41</f>
         <v>-42.299999999999727</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D45" s="13">
         <f t="shared" si="0"/>
         <v>-91.299999999999955</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45" s="13">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="F45" s="14">
+      <c r="F45" s="13">
         <f t="shared" si="0"/>
         <v>73.799999999999955</v>
       </c>
-      <c r="G45" s="14">
+      <c r="G45" s="13">
         <f t="shared" si="0"/>
         <v>-80.100000000000136</v>
       </c>
-      <c r="H45" s="14">
+      <c r="H45" s="13">
         <f t="shared" si="0"/>
         <v>-28.399999999999864</v>
       </c>
-      <c r="I45" s="14">
+      <c r="I45" s="13">
         <f t="shared" si="0"/>
         <v>-12.800000000000182</v>
       </c>
-      <c r="J45" s="14">
+      <c r="J45" s="13">
         <f t="shared" si="0"/>
         <v>30.899999999999977</v>
       </c>
-      <c r="K45" s="14">
+      <c r="K45" s="13">
         <f t="shared" si="0"/>
         <v>488.29999999999927</v>
       </c>
-      <c r="L45" s="14">
+      <c r="L45" s="13">
         <f t="shared" si="0"/>
         <v>-95.099999999999909</v>
       </c>
-      <c r="M45" s="14">
+      <c r="M45" s="13">
         <f t="shared" si="0"/>
         <v>-485.59999999999991</v>
       </c>
-      <c r="N45" s="14">
+      <c r="N45" s="13">
         <f t="shared" si="0"/>
         <v>-352.30000000000018</v>
       </c>
-      <c r="O45" s="14">
+      <c r="O45" s="13">
         <f t="shared" si="0"/>
         <v>199.59999999999991</v>
       </c>

</xml_diff>